<commit_message>
change in move file
</commit_message>
<xml_diff>
--- a/attendance_data/AI.xlsx
+++ b/attendance_data/AI.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,6 +471,11 @@
           <t>18-04-2025</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>19-04-2025</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="18.75" customHeight="1">
       <c r="A2" s="3" t="n">
@@ -632,6 +637,11 @@
           <t>P</t>
         </is>
       </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
     </row>
     <row r="28" ht="18.75" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -643,6 +653,11 @@
           <t>P</t>
         </is>
       </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
     </row>
     <row r="29" ht="18.75" customHeight="1">
       <c r="A29" s="3" t="n">
@@ -738,6 +753,11 @@
           <t>P</t>
         </is>
       </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
     </row>
     <row r="44" ht="18.75" customHeight="1">
       <c r="A44" s="3" t="n">
@@ -749,6 +769,11 @@
           <t>P</t>
         </is>
       </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
     </row>
     <row r="45" ht="18.75" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -894,6 +919,11 @@
       </c>
       <c r="B68" s="4" t="inlineStr"/>
       <c r="C68" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
         <is>
           <t>P</t>
         </is>

</xml_diff>